<commit_message>
Week 3 submission updated
Booked hours fixed and updated for everyone (Adam's original pdf was still send unchanged)
Minutes were finalized
Example of Responsibility Assignment Matrix was added to templates folder
</commit_message>
<xml_diff>
--- a/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
+++ b/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>CITS3200 Project Billed Hours Record for &lt;Zihao Liu&gt;
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Update general scope document about 'Server' and 'local database'</t>
+  </si>
+  <si>
+    <t>Create Estimation bracnch and update General Scope Work document on error handling, hardware consideration and System modle</t>
+  </si>
+  <si>
+    <t>Do Research on UML Model and hand draw our system model, then convert to digital version</t>
+  </si>
+  <si>
+    <t>Group Meeting, assigned to Project Acceptance Test Part</t>
+  </si>
+  <si>
+    <t>Create a draft of Android App of Sleep Diary</t>
   </si>
 </sst>
 </file>
@@ -243,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -269,6 +281,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -562,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -573,31 +587,31 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="71.5703125" customWidth="1"/>
+    <col min="6" max="6" width="79.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="70.5" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -618,24 +632,24 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="1"/>
@@ -658,7 +672,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
@@ -671,9 +685,9 @@
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="21"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -988,23 +1002,35 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="7" t="str">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11">
+        <v>43326</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D10" s="11">
+        <v>43326</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H10" s="1" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>9.5000000000582077</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1025,23 +1051,35 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="7" t="str">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="11">
+        <v>43326</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D11" s="11">
+        <v>43326</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H11" s="1" t="str">
+        <v>1.7499999999417923</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>11.25</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.7499999999417923</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1062,23 +1100,35 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="7" t="str">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="11">
+        <v>43327</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="D12" s="11">
+        <v>43327</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H12" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12.249999999941792</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1099,23 +1149,35 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="7" t="str">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11">
+        <v>43326</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13" s="11">
+        <v>43326</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0.875</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H13" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>13.249999999883585</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>

</xml_diff>

<commit_message>
Update weekly submission documents
</commit_message>
<xml_diff>
--- a/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
+++ b/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/null/Documents/GitHub/prof-comp/Booked_Hours/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7934E3B7-C7A1-654F-92B5-C7D8EF7B6C9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24780" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24780" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>CITS3200 Project Billed Hours Record for &lt;Zihao Liu&gt;
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -91,15 +102,18 @@
   <si>
     <t>Meet with Group, assigned task: Make a android app for questionaire</t>
   </si>
+  <si>
+    <t>Auditor Meeting</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -592,28 +606,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:F16"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="79.42578125" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="79.5" customWidth="1"/>
+    <col min="7" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" hidden="1" customWidth="1"/>
     <col min="10" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1361,23 +1375,35 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="7" t="str">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>43341</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D17" s="8">
+        <v>43341</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H17" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H17" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>18.249999999767169</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -29754,12 +29780,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10" customWidth="1"/>
   </cols>
@@ -30775,12 +30801,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Time sheet week 6
</commit_message>
<xml_diff>
--- a/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
+++ b/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>CITS3200 Project Billed Hours Record for &lt;Zihao Liu&gt;
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Add ScrollView in questionire layout, update 'AppTheme' layout file</t>
+  </si>
+  <si>
+    <t>Update layout file</t>
+  </si>
+  <si>
+    <t>Group Meeting</t>
   </si>
 </sst>
 </file>
@@ -625,8 +631,8 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1579,23 +1585,35 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="7" t="str">
+      <c r="A21" s="1">
+        <v>6</v>
+      </c>
+      <c r="B21" s="8">
+        <v>43349</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D21" s="8">
+        <v>43349</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H21" s="1" t="str">
+        <v>1.0000000001164153</v>
+      </c>
+      <c r="H21" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>23.250000000174623</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0000000001164153</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1616,23 +1634,35 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="7" t="str">
+      <c r="A22" s="1">
+        <v>6</v>
+      </c>
+      <c r="B22" s="8">
+        <v>43350</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D22" s="8">
+        <v>43350</v>
+      </c>
+      <c r="E22" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H22" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H22" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>24.250000000116415</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1653,23 +1683,35 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="7" t="str">
+      <c r="A23" s="1">
+        <v>6</v>
+      </c>
+      <c r="B23" s="8">
+        <v>43350</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D23" s="8">
+        <v>43350</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H23" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H23" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>25.250000000058208</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>

</xml_diff>

<commit_message>
update week 7 timesheet
</commit_message>
<xml_diff>
--- a/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
+++ b/Booked_Hours/Booked_Hours_Zihao_Liu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="460" windowWidth="24780" windowHeight="15600"/>
+    <workbookView xWindow="1780" yWindow="480" windowWidth="24780" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>CITS3200 Project Billed Hours Record for &lt;Zihao Liu&gt;
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Group Meeting</t>
+  </si>
+  <si>
+    <t>Meet with Joshua, demonstrate layout android studio</t>
+  </si>
+  <si>
+    <t>update qusetionire, add event listeners add date picker</t>
+  </si>
+  <si>
+    <t>Meet with auditor</t>
   </si>
 </sst>
 </file>
@@ -632,7 +641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1732,23 +1741,35 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="7" t="str">
+      <c r="A24" s="1">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8">
+        <v>43413</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D24" s="8">
+        <v>43413</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H24" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H24" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>26.25</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1769,23 +1790,35 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="7" t="str">
+      <c r="A25" s="1">
+        <v>7</v>
+      </c>
+      <c r="B25" s="8">
+        <v>43413</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="D25" s="8">
+        <v>43413</v>
+      </c>
+      <c r="E25" s="14">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H25" s="1" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="H25" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>27.75</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1806,23 +1839,35 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="7" t="str">
+      <c r="A26" s="1">
+        <v>7</v>
+      </c>
+      <c r="B26" s="8">
+        <v>43443</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D26" s="8">
+        <v>43443</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H26" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H26" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>28.749999999941792</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1843,23 +1888,35 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="7" t="str">
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="B27" s="8">
+        <v>43443</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D27" s="8">
+        <v>43443</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="7">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H27" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>29.749999999883585</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>

</xml_diff>